<commit_message>
Ajustes en las estadísticas de No Iniciados y en el Excel del Listado de Participantes Aprobados.
</commit_message>
<xml_diff>
--- a/docs/formatos/ListadoParticipantesAprobados.xlsx
+++ b/docs/formatos/ListadoParticipantesAprobados.xlsx
@@ -15,12 +15,11 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Código</t>
   </si>
@@ -64,12 +63,6 @@
     <t>Campo4</t>
   </si>
   <si>
-    <t>Fecha Inicio</t>
-  </si>
-  <si>
-    <t>Fecha Fin</t>
-  </si>
-  <si>
     <t>Promedio</t>
   </si>
   <si>
@@ -77,6 +70,18 @@
   </si>
   <si>
     <t>Empresa: YYYYYYYY</t>
+  </si>
+  <si>
+    <t>Fecha inicio</t>
+  </si>
+  <si>
+    <t>Hora inicio</t>
+  </si>
+  <si>
+    <t>Fecha fin</t>
+  </si>
+  <si>
+    <t>Hora fin</t>
   </si>
 </sst>
 </file>
@@ -249,17 +254,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,46 +588,49 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="14" width="37.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="17" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+    <row r="1" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
-    <row r="2" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
+    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
     </row>
-    <row r="3" spans="1:17" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -634,11 +642,13 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
     </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -681,17 +691,23 @@
       <c r="N4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="14" t="s">
+      <c r="O4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="14" t="s">
-        <v>15</v>
+      <c r="P4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -709,11 +725,13 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="3">
-    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O3:S3"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:N2"/>
   </mergeCells>

</xml_diff>